<commit_message>
updated model and monitor
</commit_message>
<xml_diff>
--- a/financial_models/Opportunities/Monitor/Monitor.xlsx
+++ b/financial_models/Opportunities/Monitor/Monitor.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamanl/PycharmProjects/InvestmentManagement/financial_models/Opportunities/Monitor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b10873df2abd437/Valuation - Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5A4CB4-2BC5-E243-AC43-55A9B0102B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="13_ncr:1_{C08AB8D0-CF4A-452A-99AA-E9E12773CBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD23625E-1CEE-5B41-82EC-B3159A1A15EE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opportunities" sheetId="1" r:id="rId1"/>
     <sheet name="Current_Holdings" sheetId="3" r:id="rId2"/>
-    <sheet name="Market" sheetId="4" r:id="rId3"/>
+    <sheet name="Discount rates" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Current_Holdings!$B$6:$J$6</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="98">
   <si>
     <t>Opportunities Monitor</t>
   </si>
@@ -92,6 +92,24 @@
     <t>HKG</t>
   </si>
   <si>
+    <t>1475.HK</t>
+  </si>
+  <si>
+    <t>NISSIN FOODS</t>
+  </si>
+  <si>
+    <t>1766.HK</t>
+  </si>
+  <si>
+    <t>CRRC</t>
+  </si>
+  <si>
+    <t>6186.HK</t>
+  </si>
+  <si>
+    <t>CHINA FEIHE</t>
+  </si>
+  <si>
     <t>Current Holdings Monitor</t>
   </si>
   <si>
@@ -140,21 +158,9 @@
     <t>- Expected core inflation rate (use 10Y TIPS if available) =</t>
   </si>
   <si>
-    <t>⇒ Real risk-free rate</t>
-  </si>
-  <si>
-    <t>+ Emerging Market Premium</t>
-  </si>
-  <si>
-    <t>+ Long-run ERP</t>
-  </si>
-  <si>
     <t>+ Interest Rate Risk Premium</t>
   </si>
   <si>
-    <t>⇒ Adjusted Discount rate</t>
-  </si>
-  <si>
     <t>Current Environment Assessment</t>
   </si>
   <si>
@@ -257,13 +263,7 @@
     <t>14. Recent performance/Prospective returns:</t>
   </si>
   <si>
-    <t>Cold - Weak</t>
-  </si>
-  <si>
     <t>16. Popular qualities:</t>
-  </si>
-  <si>
-    <t>Cold - "It's uninvestable"</t>
   </si>
   <si>
     <t>Capital market Sentiment</t>
@@ -315,9 +315,6 @@
     <t>1. Central bank behavior</t>
   </si>
   <si>
-    <t>Hot - Stimulative</t>
-  </si>
-  <si>
     <t>2. Inflation</t>
   </si>
   <si>
@@ -345,6 +342,61 @@
       <t>Interest rate risk premium</t>
     </r>
   </si>
+  <si>
+    <t>Equity Risk Premium</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">⇒ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Ajdusted ERP</t>
+    </r>
+  </si>
+  <si>
+    <t>+ Adjusted ERP</t>
+  </si>
+  <si>
+    <t>Hot - Positive</t>
+  </si>
+  <si>
+    <t>Mixed</t>
+  </si>
+  <si>
+    <t>Hot - Happy to hold</t>
+  </si>
+  <si>
+    <t>Mixed - "Market has bottomed"</t>
+  </si>
+  <si>
+    <t>Cold - Caution and discipline</t>
+  </si>
+  <si>
+    <t>Hot - Strong</t>
+  </si>
+  <si>
+    <t>⇒ Real risk-free rate +</t>
+  </si>
+  <si>
+    <t>Economic performance:</t>
+  </si>
+  <si>
+    <t>= Discount Rate factor</t>
+  </si>
+  <si>
+    <t>Cold - Tightening</t>
+  </si>
+  <si>
+    <t>Manual Adjustment</t>
+  </si>
 </sst>
 </file>
 
@@ -353,7 +405,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,6 +502,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -489,7 +555,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -674,43 +740,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="dotted">
         <color indexed="64"/>
@@ -721,12 +750,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -794,9 +889,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -804,9 +896,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -814,13 +903,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="8" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -829,19 +912,13 @@
     <xf numFmtId="10" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -860,10 +937,54 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="8" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="8" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="8" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -875,6 +996,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFCC"/>
       <color rgb="FFB6D7A8"/>
     </mruColors>
   </colors>
@@ -1189,7 +1312,7 @@
   <dimension ref="A2:N200"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1271,78 +1394,145 @@
         <v>16</v>
       </c>
       <c r="E5" s="7">
-        <v>3.02</v>
+        <v>2.6</v>
       </c>
       <c r="F5" s="6">
-        <v>0.1754099224177379</v>
+        <v>0.3072047302954104</v>
       </c>
       <c r="G5" s="6">
-        <v>7.4305508716723256E-2</v>
+        <v>0.13489889552202361</v>
       </c>
       <c r="H5" s="6">
         <f>F5-G5</f>
-        <v>0.10110441370101464</v>
+        <v>0.17230583477338679</v>
       </c>
       <c r="I5" s="5">
-        <v>0.34528085710129486</v>
+        <v>0.14560000000000001</v>
       </c>
       <c r="J5" s="6">
         <f>I5/E5</f>
-        <v>0.11433140963619035</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="K5" s="7">
-        <v>2</v>
+        <v>5.3</v>
       </c>
       <c r="L5" s="8">
-        <v>45001</v>
-      </c>
-      <c r="M5" s="8">
-        <v>3</v>
-      </c>
-      <c r="N5" t="b">
-        <v>1</v>
-      </c>
+        <v>44925</v>
+      </c>
+      <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="8"/>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7">
+        <v>6.54</v>
+      </c>
+      <c r="F6" s="6">
+        <v>4.981606450514553E-2</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.10891423458942941</v>
+      </c>
+      <c r="H6" s="6">
+        <f>F6-G6</f>
+        <v>-5.9098170084283877E-2</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.14560000000000001</v>
+      </c>
+      <c r="J6" s="6">
+        <f>I6/E6</f>
+        <v>2.2262996941896027E-2</v>
+      </c>
+      <c r="K6" s="7">
+        <v>5.3</v>
+      </c>
+      <c r="L6" s="8">
+        <v>45015</v>
+      </c>
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="8"/>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3.11</v>
+      </c>
+      <c r="F7" s="6">
+        <v>-0.32818777766352203</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.27236067307556133</v>
+      </c>
+      <c r="H7" s="6">
+        <f>F7-G7</f>
+        <v>-0.60054845073908336</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0.14560000000000001</v>
+      </c>
+      <c r="J7" s="6">
+        <f>I7/E7</f>
+        <v>4.6816720257234733E-2</v>
+      </c>
+      <c r="K7" s="7">
+        <v>5.3</v>
+      </c>
+      <c r="L7" s="8">
+        <v>45015</v>
+      </c>
       <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="8"/>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="7">
+        <v>6.61</v>
+      </c>
+      <c r="F8" s="6">
+        <v>-0.68464668619756364</v>
+      </c>
+      <c r="G8" s="6">
+        <v>7.1411065827984785</v>
+      </c>
+      <c r="H8" s="6">
+        <f>F8-G8</f>
+        <v>-7.8257532689960421</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0.14560000000000001</v>
+      </c>
+      <c r="J8" s="6">
+        <f>I8/E8</f>
+        <v>2.2027231467473526E-2</v>
+      </c>
+      <c r="K8" s="7">
+        <v>5.3</v>
+      </c>
+      <c r="L8" s="8">
+        <v>44925</v>
+      </c>
       <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -4062,7 +4252,7 @@
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="13" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -4070,31 +4260,31 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="52">
-        <v>44929</v>
-      </c>
-      <c r="J2" s="52"/>
+        <v>24</v>
+      </c>
+      <c r="I2" s="46">
+        <v>44902</v>
+      </c>
+      <c r="J2" s="46"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
+        <v>25</v>
+      </c>
+      <c r="D3" s="44"/>
+      <c r="E3" s="45"/>
       <c r="F3" s="12" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+        <v>27</v>
+      </c>
+      <c r="D4" s="47"/>
+      <c r="E4" s="48"/>
       <c r="F4" s="11" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -4108,32 +4298,47 @@
         <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="F7" s="7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G7" s="9">
+        <v>22000</v>
+      </c>
+      <c r="H7" s="9">
+        <f>F7*G7</f>
+        <v>50599.999999999993</v>
+      </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
@@ -6083,173 +6288,174 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB6B1BF-BEDD-44AB-AFC3-888836F1C221}">
-  <dimension ref="A2:E41"/>
+  <dimension ref="A2:F45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="137" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="2" width="62.5" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="5" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="17"/>
-      <c r="B2" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="45" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="40">
+        <v>37</v>
+      </c>
+      <c r="D3" s="37">
         <v>3.8399999999999997E-2</v>
       </c>
-      <c r="E3" s="40">
+      <c r="F3" s="37">
         <v>2.9049999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="39">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="58">
         <v>1.584E-2</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="15"/>
+      <c r="F4" s="58">
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="41">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="17"/>
+      <c r="B6" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="55">
         <f>D3-D4</f>
         <v>2.2559999999999997E-2</v>
       </c>
-      <c r="E5" s="41">
-        <f>E3-E4</f>
+      <c r="F7" s="55">
+        <f>F3-F4</f>
         <v>1.925E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="42">
-        <v>0</v>
-      </c>
-      <c r="E6" s="39">
-        <f>D3/2</f>
-        <v>1.9199999999999998E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="55">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E7" s="56"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="47">
-        <f>D41</f>
-        <v>2.0591999999999999E-2</v>
-      </c>
-      <c r="E8" s="48">
-        <f>E41</f>
-        <v>1.0001801599999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="43">
-        <f>IF(D5+D6+D7+D8&lt;6%,6%,D5+D6+D41+D7)</f>
-        <v>8.8151999999999994E-2</v>
-      </c>
-      <c r="E9" s="43">
-        <f>IF(E5+E6+E41+D7+E8&lt;6%,6%,E5+E6+E41+D7)</f>
-        <v>9.3451801599999995E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="15"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="44" t="str">
-        <f>D2</f>
+      <c r="D8" s="56">
+        <f>D45</f>
+        <v>1.7424000000000002E-2</v>
+      </c>
+      <c r="E8" s="57"/>
+      <c r="F8" s="42">
+        <f>F45</f>
+        <v>1.274E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="38">
+        <f>D37</f>
+        <v>2.8160000000000001E-2</v>
+      </c>
+      <c r="F9" s="42">
+        <f>F37</f>
+        <v>4.4966666666666662E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="39">
+        <f>IF(D7+D8+D9&lt;6%,6%,D7+D8+D9)</f>
+        <v>6.8143999999999996E-2</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="39">
+        <f>IF(F7+F8+F9&lt;6%,6%,F7+F8+F9)</f>
+        <v>7.6956666666666659E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="17"/>
+      <c r="B12" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="61" t="str">
+        <f>D6</f>
         <v>US</v>
       </c>
-      <c r="E12" s="45" t="str">
-        <f>E2</f>
+      <c r="E12" s="61"/>
+      <c r="F12" s="4" t="str">
+        <f>F6</f>
         <v>China</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="20"/>
-      <c r="B13" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="23">
-        <f t="shared" ref="C13:C16" si="0">IF(LEFT(D13,1)="H",1,IF(LEFT(D13,1)="C",-1,0))</f>
-        <v>-1</v>
-      </c>
-      <c r="D13" s="24" t="s">
+      <c r="B13" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" s="22"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="60"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="20"/>
       <c r="B14" s="22" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="23">
+        <f t="shared" ref="C14:E17" si="0">IF(LEFT(D14,1)="H",1,IF(LEFT(D14,1)="C",-1,0))</f>
+        <v>-1</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="23">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="F14" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="20"/>
       <c r="B15" s="22" t="s">
         <v>44</v>
@@ -6258,80 +6464,100 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="23">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="23">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F16" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="20"/>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="20" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="23">
-        <f>IF(LEFT(D17,1)="H",2,IF(LEFT(D17,1)="C",-1,0))</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="D17" s="29" t="str">
-        <f>IF(SUM(C13:C16)&gt;=3, "Hot", IF(SUM(C13:C16)&lt;=-3,"Cold", "Mixed"))</f>
+      <c r="D17" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="B18" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="23">
+        <f>IF(LEFT(D18,1)="H",2,IF(LEFT(D18,1)="C",-1,0))</f>
+        <v>-1</v>
+      </c>
+      <c r="D18" s="29" t="str">
+        <f>IF(SUM(C14:C17)&gt;=3, "Hot", IF(SUM(C14:C17)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Cold</v>
       </c>
-      <c r="E17" s="29" t="str">
-        <f>IF(SUM(D13:D16)&gt;=3, "Hot", IF(SUM(D13:D16)&lt;=-3,"Cold", "Mixed"))</f>
+      <c r="E18" s="23">
+        <f>IF(LEFT(F18,1)="H",2,IF(LEFT(F18,1)="C",-1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="29" t="str">
+        <f>IF(SUM(E14:E17)&gt;=3, "Hot", IF(SUM(E14:E17)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Mixed</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
-      <c r="B18" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="23">
-        <f t="shared" ref="C18:C21" si="1">IF(LEFT(D18,1)="H",1,IF(LEFT(D18,1)="C",-1,0))</f>
-        <v>-1</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="22" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="23">
+        <f t="shared" ref="C19:E22" si="1">IF(LEFT(D19,1)="H",1,IF(LEFT(D19,1)="C",-1,0))</f>
+        <v>-1</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="23">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="F19" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="20"/>
       <c r="B20" s="22" t="s">
         <v>53</v>
@@ -6340,14 +6566,18 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="23">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="F20" s="24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="22" t="s">
         <v>55</v>
@@ -6359,61 +6589,77 @@
       <c r="D21" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="22" t="s">
         <v>57</v>
       </c>
       <c r="C22" s="23">
-        <f>IF(LEFT(D22,1)="H",2,IF(LEFT(D22,1)="C",-1,0))</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="D22" s="30" t="str">
-        <f>IF(SUM(C18:C21)&gt;=3, "Hot", IF(SUM(C18:C21)&lt;=-3,"Cold", "Mixed"))</f>
+      <c r="D22" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="23">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="20"/>
+      <c r="B23" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="23">
+        <f>IF(LEFT(D23,1)="H",2,IF(LEFT(D23,1)="C",-1,0))</f>
+        <v>-1</v>
+      </c>
+      <c r="D23" s="30" t="str">
+        <f>IF(SUM(C19:C22)&gt;=3, "Hot", IF(SUM(C19:C22)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Cold</v>
       </c>
-      <c r="E22" s="30" t="str">
-        <f>IF(SUM(D18:D21)&gt;=3, "Hot", IF(SUM(D18:D21)&lt;=-3,"Cold", "Mixed"))</f>
-        <v>Mixed</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="23">
-        <f t="shared" ref="C23:C26" si="2">IF(LEFT(D23,1)="H",1,IF(LEFT(D23,1)="C",-1,0))</f>
+      <c r="E23" s="23">
+        <f>IF(LEFT(F23,1)="H",2,IF(LEFT(F23,1)="C",-1,0))</f>
         <v>-1</v>
       </c>
-      <c r="D23" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="30" t="str">
+        <f>IF(SUM(E19:E22)&gt;=3, "Hot", IF(SUM(E19:E22)&lt;=-3,"Cold", "Mixed"))</f>
+        <v>Cold</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="22" t="s">
         <v>60</v>
       </c>
       <c r="C24" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="C24:E27" si="2">IF(LEFT(D24,1)="H",1,IF(LEFT(D24,1)="C",-1,0))</f>
         <v>-1</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="23">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F24" s="24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="22" t="s">
         <v>62</v>
@@ -6425,11 +6671,15 @@
       <c r="D25" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="20"/>
       <c r="B26" s="22" t="s">
         <v>64</v>
@@ -6441,61 +6691,77 @@
       <c r="D26" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E26" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="20"/>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="22" t="s">
         <v>66</v>
       </c>
       <c r="C27" s="23">
-        <f>IF(LEFT(D27,1)="H",2,IF(LEFT(D27,1)="C",-1,0))</f>
+        <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="D27" s="30" t="str">
-        <f>IF(SUM(C23:C26)&gt;=3, "Hot", IF(SUM(C23:C26)&lt;=-3,"Cold", "Mixed"))</f>
+      <c r="D27" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="20"/>
+      <c r="B28" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="23">
+        <f>IF(LEFT(D28,1)="H",2,IF(LEFT(D28,1)="C",-1,0))</f>
+        <v>-1</v>
+      </c>
+      <c r="D28" s="30" t="str">
+        <f>IF(SUM(C24:C27)&gt;=3, "Hot", IF(SUM(C24:C27)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Cold</v>
       </c>
-      <c r="E27" s="30" t="str">
-        <f>IF(SUM(D23:D26)&gt;=3, "Hot", IF(SUM(D23:D26)&lt;=-3,"Cold", "Mixed"))</f>
+      <c r="E28" s="23">
+        <f>IF(LEFT(F28,1)="H",2,IF(LEFT(F28,1)="C",-1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="30" t="str">
+        <f>IF(SUM(E24:E27)&gt;=3, "Hot", IF(SUM(E24:E27)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Mixed</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
-      <c r="B28" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="23">
-        <f t="shared" ref="C28:C31" si="3">IF(LEFT(D28,1)="H",1,IF(LEFT(D28,1)="C",-1,0))</f>
-        <v>-1</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="20"/>
       <c r="B29" s="22" t="s">
         <v>69</v>
       </c>
       <c r="C29" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C29:E32" si="3">IF(LEFT(D29,1)="H",1,IF(LEFT(D29,1)="C",-1,0))</f>
         <v>-1</v>
       </c>
       <c r="D29" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E29" s="24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E29" s="23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="20"/>
       <c r="B30" s="22" t="s">
         <v>71</v>
@@ -6507,238 +6773,347 @@
       <c r="D30" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="E30" s="24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E30" s="23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="20"/>
       <c r="B31" s="22" t="s">
         <v>73</v>
       </c>
       <c r="C31" s="23">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="23">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="20"/>
+      <c r="B32" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="23">
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-      <c r="D31" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="20"/>
-      <c r="B32" s="28" t="s">
+      <c r="D32" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="20"/>
+      <c r="B33" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="23">
-        <f>IF(LEFT(D32,1)="H",2,IF(LEFT(D32,1)="C",-1,0))</f>
+      <c r="C33" s="23">
+        <f>IF(LEFT(D33,1)="H",2,IF(LEFT(D33,1)="C",-1,0))</f>
         <v>-1</v>
       </c>
-      <c r="D32" s="30" t="str">
-        <f>IF(SUM(C28:C31)&gt;=3, "Hot", IF(SUM(C28:C31)&lt;=-3,"Cold", "Mixed"))</f>
+      <c r="D33" s="30" t="str">
+        <f>IF(SUM(C29:C32)&gt;=3, "Hot", IF(SUM(C29:C32)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Cold</v>
       </c>
-      <c r="E32" s="30" t="str">
-        <f>IF(SUM(D28:D31)&gt;=3, "Hot", IF(SUM(D28:D31)&lt;=-3,"Cold", "Mixed"))</f>
+      <c r="E33" s="23">
+        <f>IF(LEFT(F33,1)="H",2,IF(LEFT(F33,1)="C",-1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="30" t="str">
+        <f>IF(SUM(E29:E32)&gt;=3, "Hot", IF(SUM(E29:E32)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Mixed</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
-      <c r="B33" s="36" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="20"/>
+      <c r="B34" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="C33" s="31">
-        <f>SUM(C17,C22,C27,C32)</f>
+      <c r="C34" s="50">
+        <f>SUM(C18,C23,C28,C33)</f>
         <v>-4</v>
       </c>
-      <c r="D33" s="33" t="str">
-        <f>IF(OR(C33=4,C33=-4),"Strongly disagree",IF(C33=0,"Strongly agree",IF(OR(C33=1,C33=-1),"agree",IF(OR(C33=3,C33=-3),"disagree","unclear"))))</f>
-        <v>Strongly disagree</v>
-      </c>
-      <c r="E33" s="33" t="str">
-        <f>IF(OR(D33=4,D33=-4),"Strongly disagree",IF(D33=0,"Strongly agree",IF(OR(D33=1,D33=-1),"agree",IF(OR(D33=3,D33=-3),"disagree","unclear"))))</f>
-        <v>unclear</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D34" s="32" t="str">
+        <f>IF(OR(C34=4,C34=-4),"In extreme",IF(C34=0,"In equilibrium",IF(OR(C34&gt;0),"Relatively optimistic","Relatively pessimistic")))</f>
+        <v>In extreme</v>
+      </c>
+      <c r="E34" s="50">
+        <f>SUM(E18,E23,E28,E33)</f>
+        <v>-1</v>
+      </c>
+      <c r="F34" s="32" t="str">
+        <f>IF(OR(E34=4,E34=-4),"In extreme",IF(E34=0,"In equilibrium",IF(OR(E34&gt;0),"Relatively optimistic","Relatively pessimistic")))</f>
+        <v>Relatively pessimistic</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="20"/>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="65">
+        <f>D3/1.5</f>
+        <v>2.5599999999999998E-2</v>
+      </c>
+      <c r="E35" s="51"/>
+      <c r="F35" s="65">
+        <f>(F3+D3)/1.5</f>
+        <v>4.4966666666666662E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="20"/>
+      <c r="B36" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="66">
+        <v>0</v>
+      </c>
+      <c r="E36" s="67"/>
+      <c r="F36" s="68"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="20"/>
+      <c r="B37" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="51">
+        <f>IF(C34=4,1.2, IF(C34=-4,1.1,1))</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D37" s="62">
+        <f>D35*C37*(1+D36)</f>
+        <v>2.8160000000000001E-2</v>
+      </c>
+      <c r="E37" s="64">
+        <f>IF(E34=4,1.2, IF(E34=-4,1.1,1))</f>
+        <v>1</v>
+      </c>
+      <c r="F37" s="62">
+        <f>F35*E37*(1+D36)</f>
+        <v>4.4966666666666662E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="20"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="20"/>
+      <c r="B39" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="E35" s="46" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="20"/>
-      <c r="B36" s="20" t="s">
+      <c r="C39" s="20"/>
+      <c r="D39" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" s="20"/>
+      <c r="F39" s="41" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="20"/>
+      <c r="B40" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="38">
-        <f>IF(LEFT(D36,1)="H",2,IF(LEFT(D36,1)="C",0,1))</f>
-        <v>2</v>
-      </c>
-      <c r="D36" s="27" t="s">
+      <c r="C40" s="36">
+        <f>IF(LEFT(D40,1)="H",2,IF(LEFT(D40,1)="C",0,1))</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" s="36">
+        <f>IF(LEFT(F40,1)="H",2,IF(LEFT(F40,1)="C",0,1))</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B41" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="E36" s="27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" s="38">
-        <f t="shared" ref="C37:C40" si="4">IF(LEFT(D37,1)="H",2,IF(LEFT(D37,1)="C",0,1))</f>
+      <c r="C41" s="36">
+        <f t="shared" ref="C41:E44" si="4">IF(LEFT(D41,1)="H",2,IF(LEFT(D41,1)="C",0,1))</f>
         <v>1</v>
       </c>
-      <c r="D37" s="32" t="str">
+      <c r="D41" s="31" t="str">
         <f>IF(D4&gt;=3%, "Hot - High", IF(D4&lt;=1.5%, "Cold - Low", "Mixed - Dormant"))</f>
         <v>Mixed - Dormant</v>
       </c>
-      <c r="E37" s="32" t="str">
-        <f>IF(E4&gt;=3%, "Hot - High", IF(E4&lt;=1.5%, "Cold - Low", "Mixed - Dormant"))</f>
-        <v>Cold - Low</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="38">
+      <c r="E41" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D38" s="32" t="str">
-        <f>D14</f>
-        <v>Cold - Negative</v>
-      </c>
-      <c r="E38" s="32" t="str">
-        <f>E14</f>
-        <v>Cold - Negative</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="38">
+      <c r="F41" s="31" t="str">
+        <f>IF(F4&gt;=3%, "Hot - High", IF(F4&lt;=1.5%, "Cold - Low", "Mixed - Dormant"))</f>
+        <v>Cold - Low</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B42" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D39" s="32" t="str">
-        <f>D20</f>
-        <v>Cold - High</v>
-      </c>
-      <c r="E39" s="32" t="str">
-        <f>E20</f>
-        <v>Cold - High</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="38">
+      <c r="D42" s="31" t="str">
+        <f>D15</f>
+        <v>Cold - Negative</v>
+      </c>
+      <c r="E42" s="36">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F42" s="31" t="str">
+        <f>F15</f>
+        <v>Hot - Positive</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B43" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D40" s="32" t="str">
+      <c r="D43" s="31" t="str">
         <f>D21</f>
+        <v>Cold - High</v>
+      </c>
+      <c r="E43" s="36">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F43" s="31" t="str">
+        <f>F21</f>
+        <v>Mixed</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B44" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D44" s="31" t="str">
+        <f>D22</f>
         <v>Cold - Wide</v>
       </c>
-      <c r="E40" s="32" t="str">
-        <f>E21</f>
+      <c r="E44" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="31" t="str">
+        <f>F22</f>
         <v>Cold - Wide</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" s="35">
-        <f>SUM(C36:C40)/10</f>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B45" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="52">
+        <f>SUM(C40:C44)/10</f>
+        <v>0.1</v>
+      </c>
+      <c r="D45" s="62">
+        <f>D4*(1+C45)</f>
+        <v>1.7424000000000002E-2</v>
+      </c>
+      <c r="E45" s="63">
+        <f>SUM(E40:E44)/10</f>
         <v>0.3</v>
       </c>
-      <c r="D41" s="33">
-        <f>D4*(1+C41)</f>
-        <v>2.0591999999999999E-2</v>
-      </c>
-      <c r="E41" s="33">
-        <f>E4*(1+D41)</f>
-        <v>1.0001801599999999E-2</v>
+      <c r="F45" s="62">
+        <f>F4*(1+E45)</f>
+        <v>1.274E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D36:F36"/>
   </mergeCells>
   <dataValidations count="19">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D38:E40" xr:uid="{1162B5FC-A49C-4643-AD1D-C21129BF3948}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:E16" xr:uid="{DCF9736D-3C9B-4279-B56F-4C2003DB4929}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D42:D44 F42:F44" xr:uid="{1162B5FC-A49C-4643-AD1D-C21129BF3948}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17 F17" xr:uid="{DCF9736D-3C9B-4279-B56F-4C2003DB4929}">
       <formula1>"Hot - Minimal, Cold - Rising, Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D36:E36" xr:uid="{1E460FDF-FE88-44E4-A4A8-C40EF242A498}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D40 F40" xr:uid="{1E460FDF-FE88-44E4-A4A8-C40EF242A498}">
       <formula1>"Hot - Stimulative, Cold - Tightening, Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D21:E21" xr:uid="{05972E92-5CCB-4538-80C0-0E3C4DAA650C}">
+    <dataValidation type="list" allowBlank="1" sqref="D22 F22" xr:uid="{05972E92-5CCB-4538-80C0-0E3C4DAA650C}">
       <formula1>"Hot - Narrow,Cold - Wide,Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D18:E18" xr:uid="{E29A466E-8A51-4B09-81F0-9E467356D8D5}">
+    <dataValidation type="list" allowBlank="1" sqref="D19 F19" xr:uid="{E29A466E-8A51-4B09-81F0-9E467356D8D5}">
       <formula1>"Hot - Plentiful,Cold - Scarce,Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D29:E29" xr:uid="{A3F1DC8E-57BA-4F25-894E-D6759F030FDF}">
+    <dataValidation type="list" allowBlank="1" sqref="D30 F30" xr:uid="{A3F1DC8E-57BA-4F25-894E-D6759F030FDF}">
       <formula1>"Hot - Hard to gain entry,Cold - Open to anyone,Hot - 
 New ones daily,Cold - Only the best can raise money,Hot - GP hold the cards on terms,Cold - LP have bargaining power,Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D13:E13" xr:uid="{D399A8E6-6D95-4A97-94AE-BF73E0CF82C3}">
+    <dataValidation type="list" allowBlank="1" sqref="D14 F14" xr:uid="{D399A8E6-6D95-4A97-94AE-BF73E0CF82C3}">
       <formula1>"Hot - Vibrant,Cold - Sluggish,Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D15:E15" xr:uid="{8B23EEE0-8D29-45A7-BABD-272B21016758}">
+    <dataValidation type="list" allowBlank="1" sqref="D16 F16" xr:uid="{8B23EEE0-8D29-45A7-BABD-272B21016758}">
       <formula1>"Hot - Eager,Cold - Reticent,Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D25:E25" xr:uid="{3F44EEB6-0601-492A-A711-71005020FA19}">
+    <dataValidation type="list" allowBlank="1" sqref="D26 F26" xr:uid="{3F44EEB6-0601-492A-A711-71005020FA19}">
       <formula1>"Hot - Optimistic,Cold - Pessimistic,Hot - Sanguine,Cold - Distressed,Hot - Eager to buy,Cold - Uninterested in buying,Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D24:E24" xr:uid="{01BCA93F-C7F4-4445-82F8-F61AC8C6BEF8}">
+    <dataValidation type="list" allowBlank="1" sqref="D25 F25" xr:uid="{01BCA93F-C7F4-4445-82F8-F61AC8C6BEF8}">
       <formula1>"Hot - High,Cold - Low,Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D26:E26" xr:uid="{EDC56A00-C31B-4484-B8FC-6A57C3B6D758}">
+    <dataValidation type="list" allowBlank="1" sqref="D27 F27" xr:uid="{EDC56A00-C31B-4484-B8FC-6A57C3B6D758}">
       <formula1>"Hot - Few,Cold - Many,Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D31:E31" xr:uid="{4182A36E-CA23-4874-A9A3-7EBFE34FF04E}">
+    <dataValidation type="list" allowBlank="1" sqref="D32 F32" xr:uid="{4182A36E-CA23-4874-A9A3-7EBFE34FF04E}">
       <formula1>"Hot - Aggressiveness,Cold - Caution and discipline,Hot - Broad reach,Cold - ""It's uninvestable"",Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D23:E23" xr:uid="{50DA1868-046D-4965-A766-6872EAF3DAE7}">
+    <dataValidation type="list" allowBlank="1" sqref="D24 F24" xr:uid="{50DA1868-046D-4965-A766-6872EAF3DAE7}">
       <formula1>"Hot - Happy to hold,Cold - Rushing for the exits,Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D28:E28" xr:uid="{2E90ABF5-27B6-45EA-924A-726A450132AD}">
+    <dataValidation type="list" allowBlank="1" sqref="D29 F29" xr:uid="{2E90ABF5-27B6-45EA-924A-726A450132AD}">
       <formula1>"Hot - Average person joins the market,Cold - ""Worse is yet to come"",Mixed - ""Market has bottomed"""</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D30:E30" xr:uid="{CE58FBAB-05BA-429E-979A-A80495C7634A}">
+    <dataValidation type="list" allowBlank="1" sqref="D31 F31" xr:uid="{CE58FBAB-05BA-429E-979A-A80495C7634A}">
       <formula1>"Hot - Strong,Cold - Weak,Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D14:E14" xr:uid="{80AB7CF9-33FA-49A2-857A-A16511DD9778}">
+    <dataValidation type="list" allowBlank="1" sqref="D15 F15" xr:uid="{80AB7CF9-33FA-49A2-857A-A16511DD9778}">
       <formula1>"Hot - Positive,Cold - Negative,Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D19:E19" xr:uid="{AF2B28BD-3B2E-4C4F-9341-2D3DF85E4B51}">
+    <dataValidation type="list" allowBlank="1" sqref="D20 F20" xr:uid="{AF2B28BD-3B2E-4C4F-9341-2D3DF85E4B51}">
       <formula1>"Hot - Easy,Cold - Restrictive,Mixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D20:E20" xr:uid="{CB91B3B3-F107-40CA-9A38-987E11E74D07}">
+    <dataValidation type="list" allowBlank="1" sqref="D21 F21" xr:uid="{CB91B3B3-F107-40CA-9A38-987E11E74D07}">
       <formula1>"Hot - Low,Cold - High,Mixed"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" sqref="D33:E33" xr:uid="{EA6F9DE9-1D2B-41CE-B86F-59C772E5B0CA}"/>
+    <dataValidation allowBlank="1" sqref="D34:D36 F34:F35" xr:uid="{EA6F9DE9-1D2B-41CE-B86F-59C772E5B0CA}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>